<commit_message>
link to google sheet, change column names, intitution coordinates
</commit_message>
<xml_diff>
--- a/MAP/European Network of Ethnobiology_old.xlsx
+++ b/MAP/European Network of Ethnobiology_old.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dauam-my.sharepoint.com/personal/jimena_mateo_uam_es/Documents/Documents/Estudios/Doctorado/Colaboraciones/European Network of Ethnobiology/european_ethnobiology/MAP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{DAC4F44B-79F9-4EE5-8DD7-B22CCB24A898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A821F45B-F6F3-5BC0-83BD-4809DFF6BD56}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{DAC4F44B-79F9-4EE5-8DD7-B22CCB24A898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F080D21-6DF1-1746-A3EF-F56F18DF1A76}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="1660" windowWidth="29040" windowHeight="18780" xr2:uid="{09740429-8AA6-42FE-A839-6D384F2AFAFA}"/>
   </bookViews>
@@ -25,24 +25,24 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={D96BD54D-1F9E-4000-A2D9-3F2D86B9E777}</author>
     <author>tc={02964F48-9E88-48AF-9FDF-6A2847A77599}</author>
-    <author>tc={D96BD54D-1F9E-4000-A2D9-3F2D86B9E777}</author>
   </authors>
   <commentList>
-    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{02964F48-9E88-48AF-9FDF-6A2847A77599}">
+    <comment ref="K24" authorId="0" shapeId="0" xr:uid="{D96BD54D-1F9E-4000-A2D9-3F2D86B9E777}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I do not know what to do with people based outside the EU even if politically in the EU, should we add them on a side of the map? The main map in my opinion should include only Europe</t>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="1" shapeId="0" xr:uid="{02964F48-9E88-48AF-9FDF-6A2847A77599}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I entered his French address</t>
-      </text>
-    </comment>
-    <comment ref="K9" authorId="1" shapeId="0" xr:uid="{D96BD54D-1F9E-4000-A2D9-3F2D86B9E777}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    I do not know what to do with people based outside the EU even if politically in the EU, should we add them on a side of the map? The main map in my opinion should include only Europe</t>
       </text>
     </comment>
   </commentList>
@@ -2687,27 +2687,30 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="K6" dT="2025-07-31T23:50:45.19" personId="{E2CC9E56-B7E7-47B7-BBAC-9F2800B81F57}" id="{02964F48-9E88-48AF-9FDF-6A2847A77599}">
+  <threadedComment ref="K24" dT="2025-07-31T23:52:49.48" personId="{E2CC9E56-B7E7-47B7-BBAC-9F2800B81F57}" id="{D96BD54D-1F9E-4000-A2D9-3F2D86B9E777}">
+    <text>I do not know what to do with people based outside the EU even if politically in the EU, should we add them on a side of the map? The main map in my opinion should include only Europe</text>
+  </threadedComment>
+  <threadedComment ref="K34" dT="2025-07-31T23:50:45.19" personId="{E2CC9E56-B7E7-47B7-BBAC-9F2800B81F57}" id="{02964F48-9E88-48AF-9FDF-6A2847A77599}">
     <text>I entered his French address</text>
-  </threadedComment>
-  <threadedComment ref="K9" dT="2025-07-31T23:52:49.48" personId="{E2CC9E56-B7E7-47B7-BBAC-9F2800B81F57}" id="{D96BD54D-1F9E-4000-A2D9-3F2D86B9E777}">
-    <text>I do not know what to do with people based outside the EU even if politically in the EU, should we add them on a side of the map? The main map in my opinion should include only Europe</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99047F4D-EE5C-4519-B72F-531AFA563268}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="51.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
+    <col min="8" max="8" width="51.5" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" customWidth="1"/>
     <col min="19" max="19" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2788,411 +2791,384 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>239</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>242</v>
       </c>
       <c r="H2" t="s">
-        <v>526</v>
+        <v>558</v>
       </c>
       <c r="I2" t="s">
-        <v>527</v>
+        <v>560</v>
       </c>
       <c r="J2" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P2" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>99</v>
+        <v>243</v>
+      </c>
+      <c r="R2" t="s">
+        <v>244</v>
       </c>
       <c r="S2" t="s">
         <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="U2" t="s">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="V2" t="s">
-        <v>102</v>
+        <v>245</v>
+      </c>
+      <c r="W2" t="s">
+        <v>246</v>
       </c>
       <c r="Y2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>468</v>
+        <v>446</v>
       </c>
       <c r="B3" t="s">
-        <v>469</v>
+        <v>447</v>
       </c>
       <c r="C3" t="s">
-        <v>470</v>
+        <v>448</v>
       </c>
       <c r="D3" t="s">
-        <v>471</v>
+        <v>449</v>
       </c>
       <c r="E3" t="s">
-        <v>472</v>
+        <v>450</v>
       </c>
       <c r="F3" t="s">
-        <v>473</v>
+        <v>451</v>
       </c>
       <c r="G3" t="s">
-        <v>474</v>
+        <v>452</v>
       </c>
       <c r="H3" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="I3" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="J3" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="K3" t="s">
-        <v>97</v>
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
+        <v>56</v>
       </c>
       <c r="Q3" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
       <c r="R3" t="s">
-        <v>476</v>
+        <v>454</v>
       </c>
       <c r="S3" t="s">
-        <v>477</v>
+        <v>32</v>
       </c>
       <c r="T3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="U3" t="s">
-        <v>175</v>
+        <v>214</v>
+      </c>
+      <c r="V3" t="s">
+        <v>455</v>
       </c>
       <c r="Y3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>478</v>
+        <v>328</v>
       </c>
       <c r="B4" t="s">
-        <v>479</v>
+        <v>329</v>
       </c>
       <c r="C4" t="s">
-        <v>480</v>
-      </c>
-      <c r="D4" t="s">
-        <v>481</v>
-      </c>
-      <c r="E4" t="s">
-        <v>482</v>
+        <v>330</v>
       </c>
       <c r="F4" t="s">
-        <v>483</v>
-      </c>
-      <c r="G4" t="s">
-        <v>484</v>
-      </c>
-      <c r="H4" t="s">
-        <v>526</v>
+        <v>331</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="J4" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="K4" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="P4" t="s">
-        <v>485</v>
+        <v>332</v>
       </c>
       <c r="Q4" t="s">
-        <v>485</v>
+        <v>333</v>
       </c>
       <c r="R4" t="s">
-        <v>486</v>
+        <v>334</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="T4" t="s">
-        <v>60</v>
+        <v>263</v>
       </c>
       <c r="U4" t="s">
-        <v>123</v>
-      </c>
-      <c r="V4" t="s">
-        <v>487</v>
+        <v>335</v>
+      </c>
+      <c r="W4" t="s">
+        <v>336</v>
       </c>
       <c r="Y4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>156</v>
+      </c>
+      <c r="E5" t="s">
+        <v>157</v>
       </c>
       <c r="F5" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="H5" t="s">
-        <v>528</v>
+        <v>562</v>
       </c>
       <c r="I5" t="s">
-        <v>529</v>
+        <v>561</v>
       </c>
       <c r="J5" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="K5" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>121</v>
+        <v>29</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>160</v>
       </c>
       <c r="R5" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="S5" t="s">
-        <v>85</v>
-      </c>
-      <c r="T5" t="s">
-        <v>48</v>
-      </c>
-      <c r="U5" t="s">
-        <v>123</v>
-      </c>
-      <c r="V5" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="W5" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="Y5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>253</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>256</v>
+      </c>
+      <c r="E6" t="s">
+        <v>257</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>258</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" t="s">
-        <v>530</v>
+        <v>259</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>533</v>
+        <v>555</v>
       </c>
       <c r="J6" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" t="s">
-        <v>109</v>
-      </c>
-      <c r="N6" t="s">
-        <v>111</v>
-      </c>
-      <c r="O6" t="s">
-        <v>56</v>
+        <v>260</v>
       </c>
       <c r="P6" t="s">
-        <v>109</v>
-      </c>
-      <c r="R6" t="s">
-        <v>112</v>
+        <v>261</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>262</v>
       </c>
       <c r="S6" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="T6" t="s">
-        <v>60</v>
+        <v>263</v>
       </c>
       <c r="U6" t="s">
-        <v>101</v>
+        <v>203</v>
+      </c>
+      <c r="V6" t="s">
+        <v>264</v>
       </c>
       <c r="W6" t="s">
-        <v>114</v>
+        <v>265</v>
       </c>
       <c r="Y6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>228</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="G7" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="H7" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="I7" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="J7" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="K7" t="s">
-        <v>171</v>
-      </c>
-      <c r="M7" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="P7" t="s">
-        <v>172</v>
-      </c>
-      <c r="R7" t="s">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="S7" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="T7" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="U7" t="s">
-        <v>175</v>
-      </c>
-      <c r="V7" t="s">
-        <v>176</v>
-      </c>
-      <c r="W7" t="s">
-        <v>177</v>
-      </c>
-      <c r="X7" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="Y7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
       <c r="B8" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
       <c r="C8" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E8" t="s">
-        <v>320</v>
-      </c>
-      <c r="F8" t="s">
-        <v>321</v>
+        <v>364</v>
       </c>
       <c r="G8" t="s">
-        <v>322</v>
+        <v>365</v>
       </c>
       <c r="H8" t="s">
-        <v>531</v>
+        <v>553</v>
       </c>
       <c r="I8" t="s">
-        <v>532</v>
+        <v>554</v>
       </c>
       <c r="J8" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="K8" t="s">
-        <v>171</v>
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>366</v>
       </c>
       <c r="Q8" t="s">
-        <v>323</v>
+        <v>367</v>
+      </c>
+      <c r="R8" t="s">
+        <v>368</v>
       </c>
       <c r="S8" t="s">
         <v>85</v>
       </c>
       <c r="T8" t="s">
-        <v>324</v>
+        <v>263</v>
       </c>
       <c r="U8" t="s">
-        <v>325</v>
-      </c>
-      <c r="V8" t="s">
-        <v>326</v>
-      </c>
-      <c r="W8" t="s">
-        <v>327</v>
+        <v>61</v>
       </c>
       <c r="Y8" t="s">
         <v>37</v>
@@ -3200,37 +3176,46 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>478</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>479</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>480</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>481</v>
+      </c>
+      <c r="E9" t="s">
+        <v>482</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>483</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>484</v>
+      </c>
+      <c r="H9" t="s">
+        <v>526</v>
+      </c>
+      <c r="I9" t="s">
+        <v>527</v>
       </c>
       <c r="J9" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="P9" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="Q9" t="s">
-        <v>58</v>
+        <v>485</v>
       </c>
       <c r="R9" t="s">
-        <v>59</v>
+        <v>486</v>
       </c>
       <c r="S9" t="s">
         <v>32</v>
@@ -3239,13 +3224,10 @@
         <v>60</v>
       </c>
       <c r="U9" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="V9" t="s">
-        <v>62</v>
-      </c>
-      <c r="W9" t="s">
-        <v>63</v>
+        <v>487</v>
       </c>
       <c r="Y9" t="s">
         <v>37</v>
@@ -3253,55 +3235,61 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>352</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>353</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>354</v>
+      </c>
+      <c r="E10" t="s">
+        <v>355</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>356</v>
       </c>
       <c r="H10" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="I10" t="s">
-        <v>533</v>
+        <v>542</v>
       </c>
       <c r="J10" t="s">
-        <v>568</v>
+        <v>583</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="P10" t="s">
-        <v>29</v>
+        <v>357</v>
       </c>
       <c r="Q10" t="s">
-        <v>70</v>
+        <v>358</v>
       </c>
       <c r="R10" t="s">
-        <v>71</v>
+        <v>359</v>
       </c>
       <c r="S10" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="T10" t="s">
         <v>60</v>
       </c>
       <c r="U10" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="V10" t="s">
-        <v>74</v>
+        <v>260</v>
+      </c>
+      <c r="W10" t="s">
+        <v>360</v>
       </c>
       <c r="Y10" t="s">
         <v>37</v>
@@ -3309,55 +3297,58 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>393</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>394</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>395</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>396</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>397</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>398</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>399</v>
       </c>
       <c r="H11" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="I11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J11" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="K11" t="s">
         <v>56</v>
       </c>
       <c r="P11" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>134</v>
+        <v>400</v>
       </c>
       <c r="R11" t="s">
-        <v>135</v>
+        <v>401</v>
       </c>
       <c r="S11" t="s">
-        <v>136</v>
+        <v>72</v>
+      </c>
+      <c r="T11" t="s">
+        <v>202</v>
       </c>
       <c r="U11" t="s">
-        <v>73</v>
+        <v>101</v>
+      </c>
+      <c r="V11" t="s">
+        <v>402</v>
       </c>
       <c r="W11" t="s">
-        <v>137</v>
+        <v>403</v>
       </c>
       <c r="Y11" t="s">
         <v>37</v>
@@ -3365,61 +3356,67 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>404</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>405</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>406</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>407</v>
       </c>
       <c r="E12" t="s">
-        <v>183</v>
+        <v>408</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
+        <v>409</v>
       </c>
       <c r="G12" t="s">
-        <v>185</v>
+        <v>523</v>
       </c>
       <c r="H12" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="I12" t="s">
-        <v>578</v>
+        <v>533</v>
       </c>
       <c r="J12" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="K12" t="s">
         <v>56</v>
       </c>
+      <c r="L12" t="s">
+        <v>410</v>
+      </c>
+      <c r="M12" t="s">
+        <v>411</v>
+      </c>
       <c r="P12" t="s">
-        <v>186</v>
+        <v>412</v>
       </c>
       <c r="Q12" t="s">
-        <v>187</v>
+        <v>412</v>
       </c>
       <c r="R12" t="s">
-        <v>188</v>
+        <v>413</v>
       </c>
       <c r="S12" t="s">
-        <v>32</v>
+        <v>414</v>
       </c>
       <c r="T12" t="s">
-        <v>189</v>
+        <v>324</v>
       </c>
       <c r="U12" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="V12" t="s">
-        <v>190</v>
+        <v>415</v>
       </c>
       <c r="W12" t="s">
-        <v>191</v>
+        <v>416</v>
       </c>
       <c r="Y12" t="s">
         <v>37</v>
@@ -3427,49 +3424,58 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="B13" t="s">
-        <v>229</v>
+        <v>303</v>
       </c>
       <c r="C13" t="s">
-        <v>230</v>
+        <v>304</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="E13" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="F13" t="s">
-        <v>233</v>
+        <v>307</v>
       </c>
       <c r="G13" t="s">
-        <v>234</v>
+        <v>308</v>
       </c>
       <c r="H13" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I13" t="s">
-        <v>533</v>
+        <v>580</v>
       </c>
       <c r="J13" t="s">
-        <v>568</v>
+        <v>577</v>
       </c>
       <c r="K13" t="s">
         <v>56</v>
       </c>
       <c r="P13" t="s">
-        <v>235</v>
+        <v>309</v>
+      </c>
+      <c r="R13" t="s">
+        <v>310</v>
       </c>
       <c r="S13" t="s">
-        <v>72</v>
+        <v>311</v>
       </c>
       <c r="T13" t="s">
-        <v>60</v>
+        <v>312</v>
       </c>
       <c r="U13" t="s">
-        <v>203</v>
+        <v>313</v>
+      </c>
+      <c r="V13" t="s">
+        <v>314</v>
+      </c>
+      <c r="W13" t="s">
+        <v>315</v>
       </c>
       <c r="Y13" t="s">
         <v>37</v>
@@ -3477,61 +3483,52 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>425</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>426</v>
       </c>
       <c r="C14" t="s">
-        <v>255</v>
+        <v>427</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
-      </c>
-      <c r="E14" t="s">
-        <v>257</v>
-      </c>
-      <c r="F14" t="s">
-        <v>258</v>
+        <v>428</v>
       </c>
       <c r="G14" t="s">
-        <v>259</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
+        <v>429</v>
+      </c>
+      <c r="H14" t="s">
+        <v>538</v>
       </c>
       <c r="I14" t="s">
-        <v>555</v>
+        <v>534</v>
       </c>
       <c r="J14" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="K14" t="s">
         <v>56</v>
       </c>
-      <c r="L14" t="s">
-        <v>260</v>
-      </c>
       <c r="P14" t="s">
-        <v>261</v>
+        <v>430</v>
       </c>
       <c r="Q14" t="s">
-        <v>262</v>
+        <v>431</v>
+      </c>
+      <c r="R14" t="s">
+        <v>432</v>
       </c>
       <c r="S14" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="T14" t="s">
-        <v>263</v>
+        <v>433</v>
       </c>
       <c r="U14" t="s">
-        <v>203</v>
-      </c>
-      <c r="V14" t="s">
-        <v>264</v>
+        <v>49</v>
       </c>
       <c r="W14" t="s">
-        <v>265</v>
+        <v>434</v>
       </c>
       <c r="Y14" t="s">
         <v>37</v>
@@ -3539,58 +3536,52 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>468</v>
       </c>
       <c r="B15" t="s">
-        <v>303</v>
+        <v>469</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>470</v>
       </c>
       <c r="D15" t="s">
-        <v>305</v>
+        <v>471</v>
       </c>
       <c r="E15" t="s">
-        <v>306</v>
+        <v>472</v>
       </c>
       <c r="F15" t="s">
-        <v>307</v>
+        <v>473</v>
       </c>
       <c r="G15" t="s">
-        <v>308</v>
+        <v>474</v>
       </c>
       <c r="H15" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="I15" t="s">
-        <v>580</v>
+        <v>527</v>
       </c>
       <c r="J15" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="K15" t="s">
-        <v>56</v>
-      </c>
-      <c r="P15" t="s">
-        <v>309</v>
+        <v>97</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>475</v>
       </c>
       <c r="R15" t="s">
-        <v>310</v>
+        <v>476</v>
       </c>
       <c r="S15" t="s">
-        <v>311</v>
+        <v>477</v>
       </c>
       <c r="T15" t="s">
-        <v>312</v>
+        <v>60</v>
       </c>
       <c r="U15" t="s">
-        <v>313</v>
-      </c>
-      <c r="V15" t="s">
-        <v>314</v>
-      </c>
-      <c r="W15" t="s">
-        <v>315</v>
+        <v>175</v>
       </c>
       <c r="Y15" t="s">
         <v>37</v>
@@ -3598,49 +3589,55 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="C16" t="s">
-        <v>330</v>
+        <v>280</v>
+      </c>
+      <c r="D16" t="s">
+        <v>281</v>
+      </c>
+      <c r="E16" t="s">
+        <v>282</v>
       </c>
       <c r="F16" t="s">
-        <v>331</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>534</v>
-      </c>
-      <c r="J16" t="s">
-        <v>572</v>
+        <v>283</v>
+      </c>
+      <c r="G16" t="s">
+        <v>284</v>
       </c>
       <c r="K16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" t="s">
+        <v>285</v>
+      </c>
+      <c r="M16" t="s">
         <v>56</v>
       </c>
       <c r="P16" t="s">
-        <v>332</v>
+        <v>56</v>
       </c>
       <c r="Q16" t="s">
-        <v>333</v>
+        <v>286</v>
       </c>
       <c r="R16" t="s">
-        <v>334</v>
+        <v>287</v>
       </c>
       <c r="S16" t="s">
-        <v>47</v>
+        <v>288</v>
       </c>
       <c r="T16" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="U16" t="s">
-        <v>335</v>
-      </c>
-      <c r="W16" t="s">
-        <v>336</v>
+        <v>49</v>
+      </c>
+      <c r="V16" t="s">
+        <v>290</v>
       </c>
       <c r="Y16" t="s">
         <v>37</v>
@@ -3648,61 +3645,55 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>337</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
-        <v>339</v>
+        <v>194</v>
       </c>
       <c r="D17" t="s">
-        <v>340</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
-        <v>341</v>
+        <v>196</v>
       </c>
       <c r="F17" t="s">
-        <v>342</v>
+        <v>197</v>
       </c>
       <c r="G17" t="s">
-        <v>343</v>
+        <v>198</v>
       </c>
       <c r="H17" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="I17" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="J17" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="K17" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="P17" t="s">
-        <v>344</v>
+        <v>199</v>
       </c>
       <c r="R17" t="s">
-        <v>345</v>
+        <v>200</v>
       </c>
       <c r="S17" t="s">
-        <v>346</v>
+        <v>201</v>
       </c>
       <c r="T17" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
       <c r="U17" t="s">
-        <v>347</v>
+        <v>203</v>
       </c>
       <c r="V17" t="s">
-        <v>348</v>
-      </c>
-      <c r="W17" t="s">
-        <v>349</v>
-      </c>
-      <c r="X17" t="s">
-        <v>350</v>
+        <v>204</v>
       </c>
       <c r="Y17" t="s">
         <v>37</v>
@@ -3710,58 +3701,61 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>369</v>
+        <v>337</v>
       </c>
       <c r="B18" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
       <c r="C18" t="s">
-        <v>371</v>
+        <v>339</v>
       </c>
       <c r="D18" t="s">
-        <v>372</v>
+        <v>340</v>
       </c>
       <c r="E18" t="s">
-        <v>373</v>
+        <v>341</v>
       </c>
       <c r="F18" t="s">
-        <v>374</v>
+        <v>342</v>
       </c>
       <c r="G18" t="s">
-        <v>375</v>
+        <v>343</v>
       </c>
       <c r="H18" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I18" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="J18" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="K18" t="s">
         <v>56</v>
       </c>
       <c r="P18" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>376</v>
+        <v>344</v>
       </c>
       <c r="R18" t="s">
-        <v>377</v>
+        <v>345</v>
       </c>
       <c r="S18" t="s">
-        <v>378</v>
+        <v>346</v>
       </c>
       <c r="T18" t="s">
-        <v>276</v>
+        <v>48</v>
       </c>
       <c r="U18" t="s">
-        <v>214</v>
+        <v>347</v>
+      </c>
+      <c r="V18" t="s">
+        <v>348</v>
       </c>
       <c r="W18" t="s">
-        <v>379</v>
+        <v>349</v>
+      </c>
+      <c r="X18" t="s">
+        <v>350</v>
       </c>
       <c r="Y18" t="s">
         <v>37</v>
@@ -3769,25 +3763,25 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="C19" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="D19" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="E19" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="F19" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="G19" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="H19" t="s">
         <v>540</v>
@@ -3802,25 +3796,25 @@
         <v>56</v>
       </c>
       <c r="P19" t="s">
-        <v>400</v>
+        <v>56</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>376</v>
       </c>
       <c r="R19" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="S19" t="s">
-        <v>72</v>
+        <v>378</v>
       </c>
       <c r="T19" t="s">
-        <v>202</v>
+        <v>276</v>
       </c>
       <c r="U19" t="s">
-        <v>101</v>
-      </c>
-      <c r="V19" t="s">
-        <v>402</v>
+        <v>214</v>
       </c>
       <c r="W19" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="Y19" t="s">
         <v>37</v>
@@ -3828,67 +3822,61 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>404</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>405</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>406</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>407</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>408</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>409</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>523</v>
+        <v>28</v>
       </c>
       <c r="H20" t="s">
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="I20" t="s">
-        <v>533</v>
+        <v>554</v>
       </c>
       <c r="J20" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="K20" t="s">
-        <v>56</v>
-      </c>
-      <c r="L20" t="s">
-        <v>410</v>
-      </c>
-      <c r="M20" t="s">
-        <v>411</v>
+        <v>29</v>
       </c>
       <c r="P20" t="s">
-        <v>412</v>
+        <v>30</v>
       </c>
       <c r="Q20" t="s">
-        <v>412</v>
+        <v>29</v>
       </c>
       <c r="R20" t="s">
-        <v>413</v>
+        <v>31</v>
       </c>
       <c r="S20" t="s">
-        <v>414</v>
+        <v>32</v>
       </c>
       <c r="T20" t="s">
-        <v>324</v>
+        <v>33</v>
       </c>
       <c r="U20" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="V20" t="s">
-        <v>415</v>
+        <v>35</v>
       </c>
       <c r="W20" t="s">
-        <v>416</v>
+        <v>36</v>
       </c>
       <c r="Y20" t="s">
         <v>37</v>
@@ -3896,52 +3884,58 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>425</v>
+        <v>456</v>
       </c>
       <c r="B21" t="s">
-        <v>426</v>
+        <v>457</v>
       </c>
       <c r="C21" t="s">
-        <v>427</v>
+        <v>458</v>
       </c>
       <c r="D21" t="s">
-        <v>428</v>
+        <v>459</v>
+      </c>
+      <c r="E21" t="s">
+        <v>460</v>
+      </c>
+      <c r="F21" t="s">
+        <v>461</v>
       </c>
       <c r="G21" t="s">
-        <v>429</v>
+        <v>462</v>
       </c>
       <c r="H21" t="s">
-        <v>538</v>
+        <v>563</v>
       </c>
       <c r="I21" t="s">
-        <v>534</v>
+        <v>564</v>
       </c>
       <c r="J21" t="s">
-        <v>572</v>
+        <v>587</v>
       </c>
       <c r="K21" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="P21" t="s">
-        <v>430</v>
+        <v>463</v>
       </c>
       <c r="Q21" t="s">
-        <v>431</v>
+        <v>464</v>
       </c>
       <c r="R21" t="s">
-        <v>432</v>
+        <v>465</v>
       </c>
       <c r="S21" t="s">
         <v>32</v>
       </c>
       <c r="T21" t="s">
-        <v>433</v>
+        <v>466</v>
       </c>
       <c r="U21" t="s">
-        <v>49</v>
+        <v>175</v>
       </c>
       <c r="W21" t="s">
-        <v>434</v>
+        <v>467</v>
       </c>
       <c r="Y21" t="s">
         <v>37</v>
@@ -3949,391 +3943,382 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="B22" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="C22" t="s">
-        <v>448</v>
+        <v>382</v>
       </c>
       <c r="D22" t="s">
-        <v>449</v>
-      </c>
-      <c r="E22" t="s">
-        <v>450</v>
+        <v>383</v>
       </c>
       <c r="F22" t="s">
-        <v>451</v>
+        <v>384</v>
       </c>
       <c r="G22" t="s">
-        <v>452</v>
+        <v>385</v>
       </c>
       <c r="H22" t="s">
-        <v>538</v>
+        <v>557</v>
       </c>
       <c r="I22" t="s">
-        <v>534</v>
+        <v>554</v>
       </c>
       <c r="J22" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="L22" t="s">
+        <v>386</v>
+      </c>
+      <c r="M22" t="s">
+        <v>29</v>
       </c>
       <c r="P22" t="s">
         <v>56</v>
       </c>
       <c r="Q22" t="s">
-        <v>453</v>
+        <v>387</v>
       </c>
       <c r="R22" t="s">
-        <v>454</v>
+        <v>388</v>
       </c>
       <c r="S22" t="s">
         <v>32</v>
       </c>
       <c r="T22" t="s">
-        <v>48</v>
+        <v>389</v>
       </c>
       <c r="U22" t="s">
-        <v>214</v>
+        <v>390</v>
       </c>
       <c r="V22" t="s">
-        <v>455</v>
+        <v>391</v>
+      </c>
+      <c r="W22" t="s">
+        <v>392</v>
       </c>
       <c r="Y22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="I23" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
       <c r="J23" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="K23" t="s">
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="P23" t="s">
-        <v>146</v>
+        <v>29</v>
       </c>
       <c r="Q23" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="R23" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="S23" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="T23" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="U23" t="s">
-        <v>151</v>
-      </c>
-      <c r="V23" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="Y23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>194</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>195</v>
-      </c>
-      <c r="E24" t="s">
-        <v>196</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>197</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
-        <v>198</v>
-      </c>
-      <c r="H24" t="s">
-        <v>543</v>
-      </c>
-      <c r="I24" t="s">
-        <v>544</v>
+        <v>55</v>
       </c>
       <c r="J24" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="K24" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="P24" t="s">
-        <v>199</v>
+        <v>57</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>58</v>
       </c>
       <c r="R24" t="s">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="S24" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="T24" t="s">
-        <v>202</v>
+        <v>60</v>
       </c>
       <c r="U24" t="s">
-        <v>203</v>
+        <v>61</v>
       </c>
       <c r="V24" t="s">
-        <v>204</v>
+        <v>62</v>
+      </c>
+      <c r="W24" t="s">
+        <v>63</v>
       </c>
       <c r="Y24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>351</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>352</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>353</v>
+        <v>128</v>
       </c>
       <c r="D25" t="s">
-        <v>354</v>
+        <v>129</v>
       </c>
       <c r="E25" t="s">
-        <v>355</v>
+        <v>130</v>
       </c>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="G25" t="s">
-        <v>356</v>
+        <v>132</v>
       </c>
       <c r="H25" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="I25" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="J25" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="K25" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="P25" t="s">
-        <v>357</v>
+        <v>133</v>
       </c>
       <c r="Q25" t="s">
-        <v>358</v>
+        <v>134</v>
       </c>
       <c r="R25" t="s">
-        <v>359</v>
+        <v>135</v>
       </c>
       <c r="S25" t="s">
         <v>136</v>
       </c>
-      <c r="T25" t="s">
-        <v>60</v>
-      </c>
       <c r="U25" t="s">
-        <v>175</v>
-      </c>
-      <c r="V25" t="s">
-        <v>260</v>
+        <v>73</v>
       </c>
       <c r="W25" t="s">
-        <v>360</v>
+        <v>137</v>
       </c>
       <c r="Y25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>511</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>512</v>
+        <v>237</v>
       </c>
       <c r="C26" t="s">
-        <v>513</v>
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>514</v>
-      </c>
-      <c r="E26" t="s">
-        <v>515</v>
+        <v>249</v>
       </c>
       <c r="F26" t="s">
-        <v>516</v>
+        <v>250</v>
       </c>
       <c r="G26" t="s">
-        <v>517</v>
-      </c>
-      <c r="H26" t="s">
-        <v>547</v>
-      </c>
-      <c r="I26" t="s">
-        <v>548</v>
-      </c>
-      <c r="J26" t="s">
-        <v>584</v>
+        <v>251</v>
       </c>
       <c r="K26" t="s">
-        <v>518</v>
+        <v>81</v>
+      </c>
+      <c r="P26" t="s">
+        <v>109</v>
       </c>
       <c r="Q26" t="s">
-        <v>519</v>
-      </c>
-      <c r="R26" t="s">
-        <v>520</v>
+        <v>81</v>
       </c>
       <c r="S26" t="s">
-        <v>414</v>
+        <v>252</v>
       </c>
       <c r="T26" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="U26" t="s">
-        <v>203</v>
-      </c>
-      <c r="V26" t="s">
-        <v>521</v>
-      </c>
-      <c r="W26" t="s">
-        <v>522</v>
+        <v>123</v>
       </c>
       <c r="Y26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>417</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>418</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>419</v>
+        <v>117</v>
       </c>
       <c r="D27" t="s">
-        <v>420</v>
-      </c>
-      <c r="E27" t="s">
-        <v>421</v>
+        <v>118</v>
       </c>
       <c r="F27" t="s">
-        <v>422</v>
+        <v>119</v>
       </c>
       <c r="G27" t="s">
-        <v>423</v>
+        <v>120</v>
       </c>
       <c r="H27" t="s">
-        <v>549</v>
+        <v>528</v>
       </c>
       <c r="I27" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="J27" t="s">
-        <v>585</v>
+        <v>566</v>
       </c>
       <c r="K27" t="s">
-        <v>366</v>
+        <v>121</v>
+      </c>
+      <c r="P27" t="s">
+        <v>121</v>
+      </c>
+      <c r="R27" t="s">
+        <v>122</v>
       </c>
       <c r="S27" t="s">
         <v>85</v>
       </c>
+      <c r="T27" t="s">
+        <v>48</v>
+      </c>
+      <c r="U27" t="s">
+        <v>123</v>
+      </c>
       <c r="V27" t="s">
-        <v>424</v>
+        <v>124</v>
+      </c>
+      <c r="W27" t="s">
+        <v>125</v>
       </c>
       <c r="Y27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s">
-        <v>206</v>
+        <v>267</v>
       </c>
       <c r="C28" t="s">
-        <v>207</v>
+        <v>268</v>
       </c>
       <c r="D28" t="s">
-        <v>208</v>
+        <v>269</v>
       </c>
       <c r="E28" t="s">
-        <v>209</v>
+        <v>270</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="G28" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="H28" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="I28" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="J28" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="K28" t="s">
-        <v>212</v>
+        <v>29</v>
       </c>
       <c r="P28" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="Q28" t="s">
-        <v>212</v>
+        <v>274</v>
+      </c>
+      <c r="R28" t="s">
+        <v>275</v>
       </c>
       <c r="S28" t="s">
-        <v>213</v>
+        <v>85</v>
       </c>
       <c r="T28" t="s">
-        <v>60</v>
+        <v>276</v>
       </c>
       <c r="U28" t="s">
-        <v>214</v>
+        <v>277</v>
       </c>
       <c r="W28" t="s">
         <v>215</v>
@@ -4342,419 +4327,404 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>417</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>418</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>419</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>420</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>421</v>
       </c>
       <c r="F29" t="s">
-        <v>27</v>
+        <v>422</v>
       </c>
       <c r="G29" t="s">
-        <v>28</v>
+        <v>423</v>
       </c>
       <c r="H29" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="I29" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="J29" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
       <c r="K29" t="s">
-        <v>29</v>
-      </c>
-      <c r="P29" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>29</v>
-      </c>
-      <c r="R29" t="s">
-        <v>31</v>
+        <v>366</v>
       </c>
       <c r="S29" t="s">
-        <v>32</v>
-      </c>
-      <c r="T29" t="s">
-        <v>33</v>
-      </c>
-      <c r="U29" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="V29" t="s">
-        <v>35</v>
-      </c>
-      <c r="W29" t="s">
-        <v>36</v>
+        <v>424</v>
       </c>
       <c r="Y29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>206</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
       <c r="F30" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="H30" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="I30" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="J30" t="s">
-        <v>569</v>
+        <v>586</v>
       </c>
       <c r="K30" t="s">
-        <v>29</v>
+        <v>212</v>
       </c>
       <c r="P30" t="s">
-        <v>29</v>
+        <v>212</v>
       </c>
       <c r="Q30" t="s">
-        <v>45</v>
-      </c>
-      <c r="R30" t="s">
-        <v>46</v>
+        <v>212</v>
       </c>
       <c r="S30" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="T30" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="U30" t="s">
-        <v>49</v>
+        <v>214</v>
+      </c>
+      <c r="W30" t="s">
+        <v>215</v>
       </c>
       <c r="Y30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>488</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>489</v>
       </c>
       <c r="C31" t="s">
-        <v>155</v>
+        <v>490</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>491</v>
       </c>
       <c r="E31" t="s">
-        <v>157</v>
+        <v>492</v>
       </c>
       <c r="F31" t="s">
-        <v>158</v>
+        <v>493</v>
       </c>
       <c r="G31" t="s">
-        <v>159</v>
-      </c>
-      <c r="H31" t="s">
-        <v>562</v>
-      </c>
-      <c r="I31" t="s">
-        <v>561</v>
+        <v>494</v>
       </c>
       <c r="J31" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="K31" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="P31" t="s">
-        <v>29</v>
+        <v>495</v>
       </c>
       <c r="Q31" t="s">
-        <v>160</v>
-      </c>
-      <c r="R31" t="s">
-        <v>161</v>
+        <v>496</v>
       </c>
       <c r="S31" t="s">
-        <v>162</v>
-      </c>
-      <c r="W31" t="s">
-        <v>163</v>
+        <v>497</v>
+      </c>
+      <c r="T31" t="s">
+        <v>276</v>
+      </c>
+      <c r="U31" t="s">
+        <v>226</v>
       </c>
       <c r="Y31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>216</v>
+        <v>511</v>
       </c>
       <c r="B32" t="s">
-        <v>217</v>
+        <v>512</v>
       </c>
       <c r="C32" t="s">
-        <v>218</v>
+        <v>513</v>
       </c>
       <c r="D32" t="s">
-        <v>219</v>
+        <v>514</v>
+      </c>
+      <c r="E32" t="s">
+        <v>515</v>
+      </c>
+      <c r="F32" t="s">
+        <v>516</v>
       </c>
       <c r="G32" t="s">
-        <v>220</v>
+        <v>517</v>
       </c>
       <c r="H32" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="I32" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="J32" t="s">
-        <v>569</v>
+        <v>584</v>
       </c>
       <c r="K32" t="s">
-        <v>29</v>
-      </c>
-      <c r="P32" t="s">
-        <v>221</v>
+        <v>518</v>
       </c>
       <c r="Q32" t="s">
-        <v>222</v>
+        <v>519</v>
       </c>
       <c r="R32" t="s">
-        <v>223</v>
+        <v>520</v>
       </c>
       <c r="S32" t="s">
-        <v>224</v>
+        <v>414</v>
       </c>
       <c r="T32" t="s">
-        <v>225</v>
+        <v>48</v>
       </c>
       <c r="U32" t="s">
-        <v>226</v>
+        <v>203</v>
+      </c>
+      <c r="V32" t="s">
+        <v>521</v>
       </c>
       <c r="W32" t="s">
-        <v>227</v>
+        <v>522</v>
       </c>
       <c r="Y32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>291</v>
       </c>
       <c r="B33" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>292</v>
       </c>
       <c r="D33" t="s">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="E33" t="s">
-        <v>240</v>
+        <v>294</v>
       </c>
       <c r="F33" t="s">
-        <v>241</v>
+        <v>295</v>
       </c>
       <c r="G33" t="s">
-        <v>242</v>
-      </c>
-      <c r="H33" t="s">
-        <v>558</v>
-      </c>
-      <c r="I33" t="s">
-        <v>560</v>
-      </c>
-      <c r="J33" t="s">
-        <v>575</v>
+        <v>296</v>
       </c>
       <c r="K33" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="Q33" t="s">
-        <v>243</v>
-      </c>
-      <c r="R33" t="s">
-        <v>244</v>
+        <v>297</v>
       </c>
       <c r="S33" t="s">
-        <v>32</v>
+        <v>298</v>
       </c>
       <c r="T33" t="s">
-        <v>48</v>
+        <v>263</v>
       </c>
       <c r="U33" t="s">
-        <v>175</v>
-      </c>
-      <c r="V33" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="W33" t="s">
-        <v>246</v>
+        <v>300</v>
+      </c>
+      <c r="X33" t="s">
+        <v>301</v>
       </c>
       <c r="Y33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>266</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>267</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>268</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
-        <v>269</v>
-      </c>
-      <c r="E34" t="s">
-        <v>270</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>271</v>
+        <v>107</v>
       </c>
       <c r="G34" t="s">
-        <v>272</v>
+        <v>108</v>
       </c>
       <c r="H34" t="s">
-        <v>559</v>
+        <v>530</v>
       </c>
       <c r="I34" t="s">
-        <v>560</v>
+        <v>533</v>
       </c>
       <c r="J34" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="K34" t="s">
-        <v>29</v>
+        <v>109</v>
+      </c>
+      <c r="L34" t="s">
+        <v>110</v>
+      </c>
+      <c r="M34" t="s">
+        <v>109</v>
+      </c>
+      <c r="N34" t="s">
+        <v>111</v>
+      </c>
+      <c r="O34" t="s">
+        <v>56</v>
       </c>
       <c r="P34" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>274</v>
+        <v>109</v>
       </c>
       <c r="R34" t="s">
-        <v>275</v>
+        <v>112</v>
       </c>
       <c r="S34" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="T34" t="s">
-        <v>276</v>
+        <v>60</v>
       </c>
       <c r="U34" t="s">
-        <v>277</v>
+        <v>101</v>
       </c>
       <c r="W34" t="s">
-        <v>215</v>
+        <v>114</v>
       </c>
       <c r="Y34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>361</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>362</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>363</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>364</v>
+        <v>67</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
       </c>
       <c r="G35" t="s">
-        <v>365</v>
+        <v>69</v>
       </c>
       <c r="H35" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="I35" t="s">
-        <v>554</v>
+        <v>533</v>
       </c>
       <c r="J35" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="K35" t="s">
+        <v>56</v>
+      </c>
+      <c r="P35" t="s">
         <v>29</v>
       </c>
-      <c r="P35" t="s">
-        <v>366</v>
-      </c>
       <c r="Q35" t="s">
-        <v>367</v>
+        <v>70</v>
       </c>
       <c r="R35" t="s">
-        <v>368</v>
+        <v>71</v>
       </c>
       <c r="S35" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="T35" t="s">
-        <v>263</v>
+        <v>60</v>
       </c>
       <c r="U35" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="V35" t="s">
+        <v>74</v>
       </c>
       <c r="Y35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>380</v>
+        <v>435</v>
       </c>
       <c r="B36" t="s">
-        <v>381</v>
+        <v>436</v>
       </c>
       <c r="C36" t="s">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="D36" t="s">
-        <v>383</v>
+        <v>438</v>
+      </c>
+      <c r="E36" t="s">
+        <v>439</v>
       </c>
       <c r="F36" t="s">
-        <v>384</v>
+        <v>440</v>
       </c>
       <c r="G36" t="s">
-        <v>385</v>
+        <v>441</v>
       </c>
       <c r="H36" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="I36" t="s">
         <v>554</v>
@@ -4765,450 +4735,483 @@
       <c r="K36" t="s">
         <v>29</v>
       </c>
-      <c r="L36" t="s">
-        <v>386</v>
-      </c>
-      <c r="M36" t="s">
-        <v>29</v>
-      </c>
       <c r="P36" t="s">
-        <v>56</v>
+        <v>442</v>
       </c>
       <c r="Q36" t="s">
-        <v>387</v>
+        <v>443</v>
       </c>
       <c r="R36" t="s">
-        <v>388</v>
+        <v>444</v>
       </c>
       <c r="S36" t="s">
         <v>32</v>
       </c>
       <c r="T36" t="s">
-        <v>389</v>
+        <v>60</v>
       </c>
       <c r="U36" t="s">
         <v>390</v>
       </c>
       <c r="V36" t="s">
-        <v>391</v>
-      </c>
-      <c r="W36" t="s">
-        <v>392</v>
+        <v>445</v>
       </c>
       <c r="Y36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>435</v>
+        <v>498</v>
       </c>
       <c r="B37" t="s">
-        <v>436</v>
+        <v>499</v>
       </c>
       <c r="C37" t="s">
-        <v>437</v>
+        <v>500</v>
       </c>
       <c r="D37" t="s">
-        <v>438</v>
+        <v>501</v>
       </c>
       <c r="E37" t="s">
-        <v>439</v>
-      </c>
-      <c r="F37" t="s">
-        <v>440</v>
+        <v>502</v>
       </c>
       <c r="G37" t="s">
-        <v>441</v>
-      </c>
-      <c r="H37" t="s">
-        <v>553</v>
-      </c>
-      <c r="I37" t="s">
-        <v>554</v>
-      </c>
-      <c r="J37" t="s">
-        <v>569</v>
+        <v>503</v>
       </c>
       <c r="K37" t="s">
-        <v>29</v>
+        <v>504</v>
       </c>
       <c r="P37" t="s">
-        <v>442</v>
+        <v>505</v>
       </c>
       <c r="Q37" t="s">
-        <v>443</v>
+        <v>506</v>
       </c>
       <c r="R37" t="s">
-        <v>444</v>
+        <v>507</v>
       </c>
       <c r="S37" t="s">
-        <v>32</v>
+        <v>508</v>
       </c>
       <c r="T37" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="U37" t="s">
-        <v>390</v>
+        <v>49</v>
       </c>
       <c r="V37" t="s">
-        <v>445</v>
+        <v>509</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>510</v>
       </c>
       <c r="Y37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>456</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>457</v>
+        <v>139</v>
       </c>
       <c r="C38" t="s">
-        <v>458</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
-        <v>459</v>
+        <v>141</v>
       </c>
       <c r="E38" t="s">
-        <v>460</v>
+        <v>142</v>
       </c>
       <c r="F38" t="s">
-        <v>461</v>
+        <v>143</v>
       </c>
       <c r="G38" t="s">
-        <v>462</v>
+        <v>144</v>
       </c>
       <c r="H38" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
       <c r="I38" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="J38" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="K38" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="P38" t="s">
-        <v>463</v>
+        <v>146</v>
       </c>
       <c r="Q38" t="s">
-        <v>464</v>
+        <v>147</v>
       </c>
       <c r="R38" t="s">
-        <v>465</v>
+        <v>148</v>
       </c>
       <c r="S38" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="T38" t="s">
-        <v>466</v>
+        <v>150</v>
       </c>
       <c r="U38" t="s">
-        <v>175</v>
-      </c>
-      <c r="W38" t="s">
-        <v>467</v>
+        <v>151</v>
+      </c>
+      <c r="V38" t="s">
+        <v>152</v>
       </c>
       <c r="Y38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="304" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>498</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>499</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>500</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
-        <v>501</v>
+        <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>502</v>
+        <v>94</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>503</v>
+        <v>96</v>
+      </c>
+      <c r="H39" t="s">
+        <v>526</v>
+      </c>
+      <c r="I39" t="s">
+        <v>527</v>
+      </c>
+      <c r="J39" t="s">
+        <v>565</v>
       </c>
       <c r="K39" t="s">
-        <v>504</v>
+        <v>97</v>
       </c>
       <c r="P39" t="s">
-        <v>505</v>
+        <v>98</v>
       </c>
       <c r="Q39" t="s">
-        <v>506</v>
-      </c>
-      <c r="R39" t="s">
-        <v>507</v>
+        <v>99</v>
       </c>
       <c r="S39" t="s">
-        <v>508</v>
+        <v>32</v>
       </c>
       <c r="T39" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="U39" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="V39" t="s">
-        <v>509</v>
-      </c>
-      <c r="X39" s="1" t="s">
-        <v>510</v>
+        <v>102</v>
       </c>
       <c r="Y39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>181</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>183</v>
       </c>
       <c r="F40" t="s">
-        <v>79</v>
+        <v>184</v>
       </c>
       <c r="G40" t="s">
-        <v>80</v>
+        <v>185</v>
+      </c>
+      <c r="H40" t="s">
+        <v>536</v>
+      </c>
+      <c r="I40" t="s">
+        <v>578</v>
       </c>
       <c r="J40" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="K40" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="P40" t="s">
-        <v>82</v>
+        <v>186</v>
       </c>
       <c r="Q40" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="R40" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="S40" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="T40" t="s">
-        <v>86</v>
+        <v>189</v>
       </c>
       <c r="U40" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="V40" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="W40" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="Y40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>247</v>
+        <v>164</v>
       </c>
       <c r="B41" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>249</v>
+        <v>167</v>
+      </c>
+      <c r="E41" t="s">
+        <v>168</v>
       </c>
       <c r="F41" t="s">
-        <v>250</v>
+        <v>169</v>
       </c>
       <c r="G41" t="s">
-        <v>251</v>
+        <v>170</v>
+      </c>
+      <c r="H41" t="s">
+        <v>531</v>
+      </c>
+      <c r="I41" t="s">
+        <v>532</v>
+      </c>
+      <c r="J41" t="s">
+        <v>567</v>
       </c>
       <c r="K41" t="s">
-        <v>81</v>
+        <v>171</v>
+      </c>
+      <c r="M41" t="s">
+        <v>171</v>
       </c>
       <c r="P41" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>81</v>
+        <v>172</v>
+      </c>
+      <c r="R41" t="s">
+        <v>173</v>
       </c>
       <c r="S41" t="s">
-        <v>252</v>
+        <v>32</v>
       </c>
       <c r="T41" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="U41" t="s">
-        <v>123</v>
+        <v>175</v>
+      </c>
+      <c r="V41" t="s">
+        <v>176</v>
+      </c>
+      <c r="W41" t="s">
+        <v>177</v>
+      </c>
+      <c r="X41" t="s">
+        <v>178</v>
       </c>
       <c r="Y41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="B42" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
       <c r="C42" t="s">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="D42" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
       <c r="E42" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
-        <v>283</v>
+        <v>321</v>
       </c>
       <c r="G42" t="s">
-        <v>284</v>
+        <v>322</v>
+      </c>
+      <c r="H42" t="s">
+        <v>531</v>
+      </c>
+      <c r="I42" t="s">
+        <v>532</v>
+      </c>
+      <c r="J42" t="s">
+        <v>567</v>
       </c>
       <c r="K42" t="s">
-        <v>81</v>
-      </c>
-      <c r="L42" t="s">
-        <v>285</v>
-      </c>
-      <c r="M42" t="s">
-        <v>56</v>
-      </c>
-      <c r="P42" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="Q42" t="s">
-        <v>286</v>
-      </c>
-      <c r="R42" t="s">
-        <v>287</v>
+        <v>323</v>
       </c>
       <c r="S42" t="s">
-        <v>288</v>
+        <v>85</v>
       </c>
       <c r="T42" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="U42" t="s">
-        <v>49</v>
+        <v>325</v>
       </c>
       <c r="V42" t="s">
-        <v>290</v>
+        <v>326</v>
+      </c>
+      <c r="W42" t="s">
+        <v>327</v>
       </c>
       <c r="Y42" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>291</v>
+        <v>216</v>
       </c>
       <c r="B43" t="s">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="C43" t="s">
-        <v>292</v>
+        <v>218</v>
       </c>
       <c r="D43" t="s">
-        <v>293</v>
-      </c>
-      <c r="E43" t="s">
-        <v>294</v>
-      </c>
-      <c r="F43" t="s">
-        <v>295</v>
+        <v>219</v>
       </c>
       <c r="G43" t="s">
-        <v>296</v>
+        <v>220</v>
+      </c>
+      <c r="H43" t="s">
+        <v>556</v>
+      </c>
+      <c r="I43" t="s">
+        <v>554</v>
+      </c>
+      <c r="J43" t="s">
+        <v>569</v>
       </c>
       <c r="K43" t="s">
-        <v>81</v>
+        <v>29</v>
+      </c>
+      <c r="P43" t="s">
+        <v>221</v>
       </c>
       <c r="Q43" t="s">
-        <v>297</v>
+        <v>222</v>
+      </c>
+      <c r="R43" t="s">
+        <v>223</v>
       </c>
       <c r="S43" t="s">
-        <v>298</v>
+        <v>224</v>
       </c>
       <c r="T43" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="U43" t="s">
-        <v>299</v>
+        <v>226</v>
       </c>
       <c r="W43" t="s">
-        <v>300</v>
-      </c>
-      <c r="X43" t="s">
-        <v>301</v>
+        <v>227</v>
       </c>
       <c r="Y43" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>488</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>489</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>490</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>491</v>
+        <v>77</v>
       </c>
       <c r="E44" t="s">
-        <v>492</v>
+        <v>78</v>
       </c>
       <c r="F44" t="s">
-        <v>493</v>
+        <v>79</v>
       </c>
       <c r="G44" t="s">
-        <v>494</v>
+        <v>80</v>
       </c>
       <c r="J44" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="K44" t="s">
         <v>81</v>
       </c>
       <c r="P44" t="s">
-        <v>495</v>
+        <v>82</v>
       </c>
       <c r="Q44" t="s">
-        <v>496</v>
+        <v>83</v>
+      </c>
+      <c r="R44" t="s">
+        <v>84</v>
       </c>
       <c r="S44" t="s">
-        <v>497</v>
+        <v>85</v>
       </c>
       <c r="T44" t="s">
-        <v>276</v>
+        <v>86</v>
       </c>
       <c r="U44" t="s">
-        <v>226</v>
+        <v>87</v>
+      </c>
+      <c r="V44" t="s">
+        <v>88</v>
+      </c>
+      <c r="W44" t="s">
+        <v>89</v>
       </c>
       <c r="Y44" t="s">
         <v>37</v>
@@ -5216,11 +5219,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Y44" xr:uid="{99047F4D-EE5C-4519-B72F-531AFA563268}">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="France"/>
-      </filters>
-    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y44">
+      <sortCondition ref="C1:C44"/>
+    </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y44">
     <sortCondition ref="K2:K44"/>

</xml_diff>